<commit_message>
Created plotly graph using px.scatter
</commit_message>
<xml_diff>
--- a/master_unicorns.xlsx
+++ b/master_unicorns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99B42B1-1A35-4E6F-9BA2-A5CE15465F2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B3B6A8-EC87-4941-AA8B-B6527530DAB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="12961" xr2:uid="{9F0C827A-DD62-4F4E-98D7-073EBFD16057}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2681" uniqueCount="1403">
   <si>
     <t>Bytedance</t>
   </si>
@@ -4230,9 +4230,6 @@
     <t>aka</t>
   </si>
   <si>
-    <t>Paytm</t>
-  </si>
-  <si>
     <t>JAND Inc.</t>
   </si>
   <si>
@@ -4257,16 +4254,55 @@
     <t>Plaid</t>
   </si>
   <si>
-    <t>Manbang</t>
-  </si>
-  <si>
-    <t>Bitmain</t>
-  </si>
-  <si>
-    <t>Biosplice</t>
-  </si>
-  <si>
     <t>Juul</t>
+  </si>
+  <si>
+    <t>Epic MegaGames</t>
+  </si>
+  <si>
+    <t>Nu Pagamentos S.A.</t>
+  </si>
+  <si>
+    <t>Nu Pagamentos</t>
+  </si>
+  <si>
+    <t>Think and Learn Private Limited</t>
+  </si>
+  <si>
+    <t>Think and Learn</t>
+  </si>
+  <si>
+    <t>Paytm, One97</t>
+  </si>
+  <si>
+    <t>Zhenguanyu Tech, Inc</t>
+  </si>
+  <si>
+    <t>Beijing Shenguanyu Keji Youxian Gongsi</t>
+  </si>
+  <si>
+    <t>SZ DJI Technology Co., Ltd.</t>
+  </si>
+  <si>
+    <t>DJI, Da-Jiang, Dajiang</t>
+  </si>
+  <si>
+    <t>CKO</t>
+  </si>
+  <si>
+    <t>GrabTaxi, MyTeksi</t>
+  </si>
+  <si>
+    <t>Manbang, Full Truck Alliance</t>
+  </si>
+  <si>
+    <t>Bitmain, Bite Dalu</t>
+  </si>
+  <si>
+    <t>Biosplice, Samumed</t>
+  </si>
+  <si>
+    <t>EasyVan, Huolala</t>
   </si>
 </sst>
 </file>
@@ -4306,7 +4342,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4322,6 +4358,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4347,7 +4389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4365,6 +4407,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4681,7 +4724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F8204-0EA8-47B0-88E9-BF94FDE2C09D}">
   <dimension ref="A1:H663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -4698,7 +4741,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1377</v>
@@ -4771,10 +4814,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D4" s="3">
         <v>74</v>
@@ -4797,7 +4840,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="3">
@@ -4821,10 +4864,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D6" s="3">
         <v>39</v>
@@ -4865,10 +4908,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>1387</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="6">
         <v>28.7</v>
@@ -4934,8 +4979,12 @@
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>1388</v>
+      </c>
       <c r="D11" s="3">
         <v>25</v>
       </c>
@@ -4956,8 +5005,12 @@
       <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>1390</v>
+      </c>
       <c r="D12" s="6">
         <v>16.5</v>
       </c>
@@ -4979,7 +5032,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1378</v>
+        <v>1392</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="3">
@@ -5002,8 +5055,12 @@
       <c r="A14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>1393</v>
+      </c>
       <c r="D14" s="6">
         <v>15.5</v>
       </c>
@@ -5021,11 +5078,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>1395</v>
+      </c>
       <c r="D15" s="3">
         <v>15</v>
       </c>
@@ -5068,7 +5129,9 @@
       <c r="A17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>1397</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="3">
         <v>15</v>
@@ -5134,7 +5197,9 @@
       <c r="A20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>1398</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="6">
         <v>14.3</v>
@@ -5157,7 +5222,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="6">
@@ -5225,7 +5290,7 @@
         <v>62</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="3">
@@ -5249,7 +5314,7 @@
         <v>65</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>1387</v>
+        <v>1399</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="3">
@@ -5273,7 +5338,7 @@
         <v>67</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>1388</v>
+        <v>1400</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="3">
@@ -5297,7 +5362,7 @@
         <v>69</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>1389</v>
+        <v>1401</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="3">
@@ -5386,7 +5451,9 @@
       <c r="A31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>1402</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="3">
         <v>10</v>
@@ -7874,7 +7941,7 @@
       </c>
       <c r="B144" s="7"/>
       <c r="C144" s="7" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D144" s="3">
         <v>3</v>

</xml_diff>